<commit_message>
Adjustments for first manuscript draft
</commit_message>
<xml_diff>
--- a/Yield/Yield_by_year_0N.xlsx
+++ b/Yield/Yield_by_year_0N.xlsx
@@ -416,19 +416,19 @@
         </is>
       </c>
       <c r="C2">
-        <v>5.218982356577305</v>
+        <v>5.21898235657733</v>
       </c>
       <c r="D2">
-        <v>0.337576884949384</v>
+        <v>0.3375769260293227</v>
       </c>
       <c r="E2">
-        <v>23.92539910935795</v>
+        <v>21.511472964381</v>
       </c>
       <c r="F2">
-        <v>4.522142928625882</v>
+        <v>4.517967691790099</v>
       </c>
       <c r="G2">
-        <v>5.915821784528728</v>
+        <v>5.919997021364561</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -451,19 +451,19 @@
         </is>
       </c>
       <c r="C3">
-        <v>7.464574684069095</v>
+        <v>7.464574684069104</v>
       </c>
       <c r="D3">
-        <v>0.3375768849493844</v>
+        <v>0.3375769260293215</v>
       </c>
       <c r="E3">
-        <v>23.92539910935795</v>
+        <v>21.51147296438204</v>
       </c>
       <c r="F3">
-        <v>6.767735256117671</v>
+        <v>6.763560019281877</v>
       </c>
       <c r="G3">
-        <v>8.16141411202052</v>
+        <v>8.165589348856331</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -486,19 +486,19 @@
         </is>
       </c>
       <c r="C4">
-        <v>5.27558953566659</v>
+        <v>5.27558953566662</v>
       </c>
       <c r="D4">
-        <v>0.6000410333339674</v>
+        <v>0.6000400152698083</v>
       </c>
       <c r="E4">
-        <v>18.63569086041779</v>
+        <v>16.44637937837114</v>
       </c>
       <c r="F4">
-        <v>4.018025429883714</v>
+        <v>4.006361686860882</v>
       </c>
       <c r="G4">
-        <v>6.533153641449466</v>
+        <v>6.544817384472357</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -521,19 +521,19 @@
         </is>
       </c>
       <c r="C5">
-        <v>7.790703678333339</v>
+        <v>7.790703678333328</v>
       </c>
       <c r="D5">
-        <v>0.6000410333339654</v>
+        <v>0.6000400152698085</v>
       </c>
       <c r="E5">
-        <v>18.63569086041764</v>
+        <v>16.44637937837151</v>
       </c>
       <c r="F5">
-        <v>6.533139572550468</v>
+        <v>6.521475829527592</v>
       </c>
       <c r="G5">
-        <v>9.048267784116211</v>
+        <v>9.059931527139064</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -556,19 +556,19 @@
         </is>
       </c>
       <c r="C6">
-        <v>4.175905373052968</v>
+        <v>4.175905373052956</v>
       </c>
       <c r="D6">
-        <v>0.7532527634446484</v>
+        <v>0.7532527608297563</v>
       </c>
       <c r="E6">
-        <v>23.40073543777808</v>
+        <v>23.40073583718799</v>
       </c>
       <c r="F6">
-        <v>2.619158537961488</v>
+        <v>2.619158544809541</v>
       </c>
       <c r="G6">
-        <v>5.732652208144449</v>
+        <v>5.732652201296371</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -591,19 +591,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>8.125867857332867</v>
+        <v>8.125867857332864</v>
       </c>
       <c r="D7">
-        <v>0.7532527634446476</v>
+        <v>0.7532527608297541</v>
       </c>
       <c r="E7">
-        <v>23.40073543777845</v>
+        <v>23.40073583718769</v>
       </c>
       <c r="F7">
-        <v>6.56912102224139</v>
+        <v>6.569121029089453</v>
       </c>
       <c r="G7">
-        <v>9.682614692424345</v>
+        <v>9.682614685576276</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -626,19 +626,19 @@
         </is>
       </c>
       <c r="C8">
-        <v>4.890159088432363</v>
+        <v>4.890159088432354</v>
       </c>
       <c r="D8">
-        <v>0.3740201134400171</v>
+        <v>0.3726900639192939</v>
       </c>
       <c r="E8">
-        <v>67.16792723145292</v>
+        <v>59.09356675379004</v>
       </c>
       <c r="F8">
-        <v>4.143646124750926</v>
+        <v>4.144432698497401</v>
       </c>
       <c r="G8">
-        <v>5.636672052113801</v>
+        <v>5.635885478367308</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -661,19 +661,19 @@
         </is>
       </c>
       <c r="C9">
-        <v>7.793715406578425</v>
+        <v>7.793715406578436</v>
       </c>
       <c r="D9">
-        <v>0.3740201134400167</v>
+        <v>0.3726900639192933</v>
       </c>
       <c r="E9">
-        <v>67.16792723145232</v>
+        <v>59.09356675379071</v>
       </c>
       <c r="F9">
-        <v>7.047202442896988</v>
+        <v>7.047989016643485</v>
       </c>
       <c r="G9">
-        <v>8.540228370259861</v>
+        <v>8.539441796513387</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>

</xml_diff>